<commit_message>
Ajustes de los KPI y ajustes gráficos finales
</commit_message>
<xml_diff>
--- a/data/crudos/insc_carreras_2026.xlsx
+++ b/data/crudos/insc_carreras_2026.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
   <si>
     <t>Año Académico</t>
   </si>
@@ -59,30 +59,36 @@
     <t>Modalidad</t>
   </si>
   <si>
+    <t>BACHI, MAIRA ALEJANDRA</t>
+  </si>
+  <si>
+    <t>DNI 36323525</t>
+  </si>
+  <si>
+    <t>2021-V1</t>
+  </si>
+  <si>
+    <t>01/10/2025</t>
+  </si>
+  <si>
+    <t>01/04/2026</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Con Título Secundario</t>
+  </si>
+  <si>
+    <t>Presencial</t>
+  </si>
+  <si>
     <t>FERNANDEZ, ROCIO ABIGAIL</t>
   </si>
   <si>
     <t>DNI 48807202</t>
   </si>
   <si>
-    <t>2021-V1</t>
-  </si>
-  <si>
-    <t>01/10/2025</t>
-  </si>
-  <si>
-    <t>01/04/2026</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>Con Título Secundario</t>
-  </si>
-  <si>
-    <t>Presencial</t>
-  </si>
-  <si>
     <t>NIEVA, MARCOS</t>
   </si>
   <si>
@@ -101,6 +107,18 @@
     <t>DNI 48639486</t>
   </si>
   <si>
+    <t>Retamozo, Nadia</t>
+  </si>
+  <si>
+    <t>DNI 34576075</t>
+  </si>
+  <si>
+    <t>Scatassa, Bruno</t>
+  </si>
+  <si>
+    <t>DNI 44511731</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cantidad de filas: </t>
   </si>
   <si>
@@ -116,6 +134,12 @@
     <t>Aceptado</t>
   </si>
   <si>
+    <t>BARRERA TITO, PAUL WILLIAM</t>
+  </si>
+  <si>
+    <t>DNI 46695130</t>
+  </si>
+  <si>
     <t>BASTAZO, DAIANA AYELEN</t>
   </si>
   <si>
@@ -134,18 +158,36 @@
     <t>DNI 37987557</t>
   </si>
   <si>
+    <t>BRAVO, MAIA FLORENCIA</t>
+  </si>
+  <si>
+    <t>DNI 43094818</t>
+  </si>
+  <si>
     <t>BURGAT CARADONNA, EZEQUIEL</t>
   </si>
   <si>
     <t>DNI 48241477</t>
   </si>
   <si>
+    <t>CARRIZO, SANTIAGO AGUSTIN</t>
+  </si>
+  <si>
+    <t>DNI 40126665</t>
+  </si>
+  <si>
     <t>CARUSO, SANTIAGO</t>
   </si>
   <si>
     <t>DNI 48161555</t>
   </si>
   <si>
+    <t>CAVALLARO, CONSTANTINO VITO</t>
+  </si>
+  <si>
+    <t>DNI 48115749</t>
+  </si>
+  <si>
     <t>DÍAZ, MELANIE MILAGROS</t>
   </si>
   <si>
@@ -170,6 +212,12 @@
     <t>DNI 46027745</t>
   </si>
   <si>
+    <t>FERNANDEZ, CANDELA CELESTE</t>
+  </si>
+  <si>
+    <t>DNI 44626514</t>
+  </si>
+  <si>
     <t>FERNANDEZ SALCH, ROMAN</t>
   </si>
   <si>
@@ -194,12 +242,24 @@
     <t>DNI 48677855</t>
   </si>
   <si>
+    <t>GERES, BIANCA TAMARA</t>
+  </si>
+  <si>
+    <t>DNI 48510323</t>
+  </si>
+  <si>
     <t>GHIGLIERI, LUKA MATEO</t>
   </si>
   <si>
     <t>DNI 46737801</t>
   </si>
   <si>
+    <t>GODOY, CLARA DANIELA</t>
+  </si>
+  <si>
+    <t>DNI 47881730</t>
+  </si>
+  <si>
     <t>GODOY OSIANI, JULIAN MANUEL</t>
   </si>
   <si>
@@ -230,6 +290,12 @@
     <t>DNI 48796378</t>
   </si>
   <si>
+    <t>LEMOS GONZÁLEZ, BRENDA CRISTAL</t>
+  </si>
+  <si>
+    <t>DNI 41075924</t>
+  </si>
+  <si>
     <t>LIZONDO ORTIGOZA, JONATHAN ARIEL</t>
   </si>
   <si>
@@ -254,6 +320,12 @@
     <t>DNI 47066576</t>
   </si>
   <si>
+    <t>MARTINEZ MOREL, LUZ MARINA</t>
+  </si>
+  <si>
+    <t>DNI 47869709</t>
+  </si>
+  <si>
     <t>MATILLA, SOFIA</t>
   </si>
   <si>
@@ -266,6 +338,12 @@
     <t>DNI 48521116</t>
   </si>
   <si>
+    <t>MONTEVERDE, JULIETA</t>
+  </si>
+  <si>
+    <t>DNI 46346107</t>
+  </si>
+  <si>
     <t>MORINIGO, LUJAN ANTONELA</t>
   </si>
   <si>
@@ -326,12 +404,24 @@
     <t>DNI 47871987</t>
   </si>
   <si>
+    <t>PRADO, MARTÍN GABRIEL</t>
+  </si>
+  <si>
+    <t>DNI 47572317</t>
+  </si>
+  <si>
     <t>PRIETO, SANTIAGO</t>
   </si>
   <si>
     <t>DNI 48240193</t>
   </si>
   <si>
+    <t>RODRIGUEZ, MAXIMO AGUSTIN</t>
+  </si>
+  <si>
+    <t>DNI 47805235</t>
+  </si>
+  <si>
     <t>ROMERO, NAHUEL EZEQUIEL</t>
   </si>
   <si>
@@ -350,6 +440,12 @@
     <t>DNI 48461926</t>
   </si>
   <si>
+    <t>SCHLAIN, TALIA NAOMI</t>
+  </si>
+  <si>
+    <t>DNI 44162493</t>
+  </si>
+  <si>
     <t>SENESI SCHIAVONE, MORENA</t>
   </si>
   <si>
@@ -374,6 +470,12 @@
     <t>DNI 46737943</t>
   </si>
   <si>
+    <t>VILLAFAÑEZ, MARÍA JULIETA</t>
+  </si>
+  <si>
+    <t>DNI 46990398</t>
+  </si>
+  <si>
     <t>VILLALBA, MARIA AGUSTINA</t>
   </si>
   <si>
@@ -399,6 +501,12 @@
   </si>
   <si>
     <t>DNI 38458463</t>
+  </si>
+  <si>
+    <t>GUEVARA, MARTIN</t>
+  </si>
+  <si>
+    <t>DNI 44498874</t>
   </si>
   <si>
     <t>JAIME, KEVIN</t>
@@ -844,10 +952,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I141" sqref="I141"/>
+      <selection activeCell="I177" sqref="I177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1059,157 +1167,157 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7">
-        <f>ROWS(A6:I9)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" customHeight="1" ht="20">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7">
+        <f>ROWS(A6:I12)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" customHeight="1" ht="20">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="6">
-        <v>2013</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="6">
-        <v>2013</v>
-      </c>
-      <c r="D14" s="6">
-        <v>2</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2013</v>
-      </c>
-      <c r="D15" s="6">
-        <v>2</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="6">
         <v>2013</v>
       </c>
@@ -1223,7 +1331,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>20</v>
@@ -1234,10 +1342,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="6" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C17" s="6">
         <v>2013</v>
@@ -1252,7 +1360,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>20</v>
@@ -1263,10 +1371,10 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="6">
         <v>2013</v>
@@ -1281,7 +1389,7 @@
         <v>18</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>20</v>
@@ -1292,10 +1400,10 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="6">
         <v>2013</v>
@@ -1310,7 +1418,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>20</v>
@@ -1321,10 +1429,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="6">
         <v>2013</v>
@@ -1339,7 +1447,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>20</v>
@@ -1350,10 +1458,10 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="6">
         <v>2013</v>
@@ -1368,7 +1476,7 @@
         <v>18</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>20</v>
@@ -1379,10 +1487,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="6">
         <v>2013</v>
@@ -1397,7 +1505,7 @@
         <v>18</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>20</v>
@@ -1408,10 +1516,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C23" s="6">
         <v>2013</v>
@@ -1426,7 +1534,7 @@
         <v>18</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>20</v>
@@ -1455,7 +1563,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>20</v>
@@ -1484,7 +1592,7 @@
         <v>18</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>20</v>
@@ -1513,7 +1621,7 @@
         <v>18</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>20</v>
@@ -1542,7 +1650,7 @@
         <v>18</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>20</v>
@@ -1571,7 +1679,7 @@
         <v>18</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>20</v>
@@ -1600,7 +1708,7 @@
         <v>18</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>20</v>
@@ -1629,7 +1737,7 @@
         <v>18</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>20</v>
@@ -1658,7 +1766,7 @@
         <v>18</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>20</v>
@@ -1669,10 +1777,10 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="6" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C32" s="6">
         <v>2013</v>
@@ -1687,7 +1795,7 @@
         <v>18</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>20</v>
@@ -1698,10 +1806,10 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C33" s="6">
         <v>2013</v>
@@ -1716,7 +1824,7 @@
         <v>18</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>20</v>
@@ -1727,10 +1835,10 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C34" s="6">
         <v>2013</v>
@@ -1745,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>20</v>
@@ -1756,10 +1864,10 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="6">
         <v>2013</v>
@@ -1774,7 +1882,7 @@
         <v>18</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>20</v>
@@ -1785,10 +1893,10 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C36" s="6">
         <v>2013</v>
@@ -1803,7 +1911,7 @@
         <v>18</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>20</v>
@@ -1814,10 +1922,10 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="6">
         <v>2013</v>
@@ -1832,7 +1940,7 @@
         <v>18</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>20</v>
@@ -1843,10 +1951,10 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C38" s="6">
         <v>2013</v>
@@ -1861,7 +1969,7 @@
         <v>18</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>20</v>
@@ -1872,10 +1980,10 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" s="6">
         <v>2013</v>
@@ -1890,7 +1998,7 @@
         <v>18</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>20</v>
@@ -1901,10 +2009,10 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C40" s="6">
         <v>2013</v>
@@ -1919,7 +2027,7 @@
         <v>18</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>20</v>
@@ -1930,10 +2038,10 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="6" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="C41" s="6">
         <v>2013</v>
@@ -1948,7 +2056,7 @@
         <v>18</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>20</v>
@@ -1977,7 +2085,7 @@
         <v>18</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>20</v>
@@ -1988,10 +2096,10 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="6" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="C43" s="6">
         <v>2013</v>
@@ -2006,7 +2114,7 @@
         <v>18</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>20</v>
@@ -2017,10 +2125,10 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="6">
         <v>2013</v>
@@ -2035,7 +2143,7 @@
         <v>18</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>20</v>
@@ -2046,10 +2154,10 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C45" s="6">
         <v>2013</v>
@@ -2064,7 +2172,7 @@
         <v>18</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>20</v>
@@ -2075,10 +2183,10 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C46" s="6">
         <v>2013</v>
@@ -2093,7 +2201,7 @@
         <v>18</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>20</v>
@@ -2104,10 +2212,10 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" s="6">
         <v>2013</v>
@@ -2122,7 +2230,7 @@
         <v>18</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>20</v>
@@ -2133,10 +2241,10 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C48" s="6">
         <v>2013</v>
@@ -2151,7 +2259,7 @@
         <v>18</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>20</v>
@@ -2162,10 +2270,10 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="6" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C49" s="6">
         <v>2013</v>
@@ -2180,7 +2288,7 @@
         <v>18</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>20</v>
@@ -2191,10 +2299,10 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C50" s="6">
         <v>2013</v>
@@ -2209,7 +2317,7 @@
         <v>18</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>20</v>
@@ -2220,10 +2328,10 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C51" s="6">
         <v>2013</v>
@@ -2238,7 +2346,7 @@
         <v>18</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>20</v>
@@ -2249,10 +2357,10 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="6" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C52" s="6">
         <v>2013</v>
@@ -2267,7 +2375,7 @@
         <v>18</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>20</v>
@@ -2278,10 +2386,10 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C53" s="6">
         <v>2013</v>
@@ -2296,7 +2404,7 @@
         <v>18</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>20</v>
@@ -2307,10 +2415,10 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="6" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C54" s="6">
         <v>2013</v>
@@ -2325,7 +2433,7 @@
         <v>18</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>20</v>
@@ -2336,10 +2444,10 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="6" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="C55" s="6">
         <v>2013</v>
@@ -2354,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>20</v>
@@ -2365,10 +2473,10 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C56" s="6">
         <v>2013</v>
@@ -2383,7 +2491,7 @@
         <v>18</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>20</v>
@@ -2394,10 +2502,10 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="6" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="C57" s="6">
         <v>2013</v>
@@ -2412,7 +2520,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>20</v>
@@ -2441,7 +2549,7 @@
         <v>18</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>20</v>
@@ -2470,7 +2578,7 @@
         <v>18</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>20</v>
@@ -2499,7 +2607,7 @@
         <v>18</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>20</v>
@@ -2528,7 +2636,7 @@
         <v>18</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>20</v>
@@ -2557,7 +2665,7 @@
         <v>18</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>20</v>
@@ -2567,75 +2675,104 @@
       </c>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7">
-        <f>ROWS(A13:I62)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" customHeight="1" ht="20">
-      <c r="A64" s="4" t="s">
+      <c r="B63" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" s="6">
+        <v>2013</v>
+      </c>
+      <c r="D63" s="6">
+        <v>2</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
+      <c r="B64" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="6">
+        <v>2013</v>
+      </c>
+      <c r="D64" s="6">
+        <v>2</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>13</v>
+      <c r="A65" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="6">
+        <v>2013</v>
+      </c>
+      <c r="D65" s="6">
+        <v>2</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C66" s="6">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="D66" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>17</v>
@@ -2644,7 +2781,7 @@
         <v>18</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>20</v>
@@ -2655,16 +2792,16 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C67" s="6">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="D67" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>17</v>
@@ -2673,7 +2810,7 @@
         <v>18</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>20</v>
@@ -2684,16 +2821,16 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C68" s="6">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="D68" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>17</v>
@@ -2702,7 +2839,7 @@
         <v>18</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>20</v>
@@ -2713,16 +2850,16 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="6" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>131</v>
+        <v>31</v>
       </c>
       <c r="C69" s="6">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="D69" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>17</v>
@@ -2731,7 +2868,7 @@
         <v>18</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>20</v>
@@ -2742,16 +2879,16 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C70" s="6">
-        <v>1</v>
+        <v>2013</v>
       </c>
       <c r="D70" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>17</v>
@@ -2760,7 +2897,7 @@
         <v>18</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>20</v>
@@ -2770,72 +2907,101 @@
       </c>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7">
-        <f>ROWS(A66:I70)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" customHeight="1" ht="20">
-      <c r="A72" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
+      <c r="A71" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="6">
+        <v>2013</v>
+      </c>
+      <c r="D71" s="6">
+        <v>2</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" s="6">
+        <v>2013</v>
+      </c>
+      <c r="D72" s="6">
+        <v>2</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>13</v>
+      <c r="A73" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" s="6">
+        <v>2013</v>
+      </c>
+      <c r="D73" s="6">
+        <v>2</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="6" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="C74" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D74" s="6">
         <v>2</v>
@@ -2847,22 +3013,24 @@
         <v>18</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H74" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="I74" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="6" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="C75" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D75" s="6">
         <v>2</v>
@@ -2874,7 +3042,7 @@
         <v>18</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>20</v>
@@ -2885,13 +3053,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="6" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="C76" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D76" s="6">
         <v>2</v>
@@ -2903,7 +3071,7 @@
         <v>18</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>20</v>
@@ -2914,13 +3082,13 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="6" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="C77" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D77" s="6">
         <v>2</v>
@@ -2932,7 +3100,7 @@
         <v>18</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>20</v>
@@ -2943,13 +3111,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="6" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="C78" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D78" s="6">
         <v>2</v>
@@ -2961,7 +3129,7 @@
         <v>18</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>20</v>
@@ -2972,13 +3140,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="6" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="C79" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D79" s="6">
         <v>2</v>
@@ -2990,7 +3158,7 @@
         <v>18</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>20</v>
@@ -3001,13 +3169,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="6" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C80" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D80" s="6">
         <v>2</v>
@@ -3019,7 +3187,7 @@
         <v>18</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>20</v>
@@ -3030,13 +3198,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="6" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="C81" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D81" s="6">
         <v>2</v>
@@ -3048,7 +3216,7 @@
         <v>18</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>20</v>
@@ -3059,13 +3227,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="6" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="C82" s="6">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D82" s="6">
         <v>2</v>
@@ -3077,7 +3245,7 @@
         <v>18</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>20</v>
@@ -3087,104 +3255,75 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C83" s="6">
-        <v>2015</v>
-      </c>
-      <c r="D83" s="6">
-        <v>2</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I83" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C84" s="6">
-        <v>2015</v>
-      </c>
-      <c r="D84" s="6">
-        <v>2</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I84" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="A83" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7">
+        <f>ROWS(A16:I82)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" customHeight="1" ht="20">
+      <c r="A84" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="6">
-        <v>2015</v>
-      </c>
-      <c r="D85" s="6">
-        <v>2</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I85" s="6" t="s">
-        <v>21</v>
+      <c r="A85" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="6" t="s">
-        <v>65</v>
+        <v>158</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="C86" s="6">
-        <v>2015</v>
+        <v>1</v>
       </c>
       <c r="D86" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>17</v>
@@ -3193,7 +3332,7 @@
         <v>18</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>20</v>
@@ -3204,16 +3343,16 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="6" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="C87" s="6">
-        <v>2015</v>
+        <v>1</v>
       </c>
       <c r="D87" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>17</v>
@@ -3222,7 +3361,7 @@
         <v>18</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>20</v>
@@ -3233,16 +3372,16 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="6" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="C88" s="6">
-        <v>2015</v>
+        <v>1</v>
       </c>
       <c r="D88" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>17</v>
@@ -3251,7 +3390,7 @@
         <v>18</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>20</v>
@@ -3262,16 +3401,16 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="6" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="C89" s="6">
-        <v>2015</v>
+        <v>1</v>
       </c>
       <c r="D89" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>17</v>
@@ -3280,7 +3419,7 @@
         <v>18</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>20</v>
@@ -3291,16 +3430,16 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="6" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="C90" s="6">
-        <v>2015</v>
+        <v>1</v>
       </c>
       <c r="D90" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>17</v>
@@ -3309,7 +3448,7 @@
         <v>18</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H90" s="6" t="s">
         <v>20</v>
@@ -3320,16 +3459,16 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="6" t="s">
-        <v>79</v>
+        <v>168</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="C91" s="6">
-        <v>2015</v>
+        <v>1</v>
       </c>
       <c r="D91" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>17</v>
@@ -3338,7 +3477,7 @@
         <v>18</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H91" s="6" t="s">
         <v>20</v>
@@ -3348,98 +3487,69 @@
       </c>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C92" s="6">
-        <v>2015</v>
-      </c>
-      <c r="D92" s="6">
-        <v>2</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H92" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I92" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C93" s="6">
-        <v>2015</v>
-      </c>
-      <c r="D93" s="6">
-        <v>2</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H93" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I93" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="A92" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7">
+        <f>ROWS(A86:I91)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" customHeight="1" ht="20">
+      <c r="A93" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C94" s="6">
-        <v>2015</v>
-      </c>
-      <c r="D94" s="6">
-        <v>2</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G94" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H94" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I94" s="6" t="s">
-        <v>21</v>
+      <c r="A94" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="6" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>90</v>
+        <v>172</v>
       </c>
       <c r="C95" s="6">
         <v>2015</v>
@@ -3456,19 +3566,17 @@
       <c r="G95" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H95" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="H95" s="6"/>
       <c r="I95" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="6" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C96" s="6">
         <v>2015</v>
@@ -3494,10 +3602,10 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="6" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
       <c r="C97" s="6">
         <v>2015</v>
@@ -3523,10 +3631,10 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="6" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="C98" s="6">
         <v>2015</v>
@@ -3552,10 +3660,10 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="6" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="C99" s="6">
         <v>2015</v>
@@ -3581,10 +3689,10 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="6" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="C100" s="6">
         <v>2015</v>
@@ -3610,10 +3718,10 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="6" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C101" s="6">
         <v>2015</v>
@@ -3639,10 +3747,10 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="6" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="C102" s="6">
         <v>2015</v>
@@ -3668,10 +3776,10 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="6" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="C103" s="6">
         <v>2015</v>
@@ -3697,10 +3805,10 @@
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="6" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="C104" s="6">
         <v>2015</v>
@@ -3726,10 +3834,10 @@
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="6" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="C105" s="6">
         <v>2015</v>
@@ -3755,10 +3863,10 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="6" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C106" s="6">
         <v>2015</v>
@@ -3783,69 +3891,98 @@
       </c>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="7">
-        <f>ROWS(A74:I106)</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" customHeight="1" ht="20">
-      <c r="A108" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
-      <c r="I108" s="4"/>
+      <c r="A107" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C107" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D107" s="6">
+        <v>2</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I107" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C108" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D108" s="6">
+        <v>2</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H108" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I108" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G109" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H109" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I109" s="5" t="s">
-        <v>13</v>
+      <c r="A109" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C109" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D109" s="6">
+        <v>2</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I109" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="6" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="C110" s="6">
         <v>2015</v>
@@ -3871,10 +4008,10 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="6" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C111" s="6">
         <v>2015</v>
@@ -3900,10 +4037,10 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="6" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C112" s="6">
         <v>2015</v>
@@ -3929,10 +4066,10 @@
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="6" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="C113" s="6">
         <v>2015</v>
@@ -3958,10 +4095,10 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="6" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="C114" s="6">
         <v>2015</v>
@@ -3987,10 +4124,10 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="6" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="C115" s="6">
         <v>2015</v>
@@ -4016,10 +4153,10 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="6" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C116" s="6">
         <v>2015</v>
@@ -4045,10 +4182,10 @@
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C117" s="6">
         <v>2015</v>
@@ -4074,10 +4211,10 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="6" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C118" s="6">
         <v>2015</v>
@@ -4102,75 +4239,104 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B119" s="7"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="7"/>
-      <c r="I119" s="7">
-        <f>ROWS(A110:I118)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" customHeight="1" ht="20">
-      <c r="A120" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
+      <c r="A119" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C119" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D119" s="6">
+        <v>2</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H119" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C120" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D120" s="6">
+        <v>2</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H120" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I120" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G121" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H121" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I121" s="5" t="s">
-        <v>13</v>
+      <c r="A121" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C121" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D121" s="6">
+        <v>2</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H121" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I121" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="6" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>141</v>
+        <v>120</v>
+      </c>
+      <c r="C122" s="6">
+        <v>2015</v>
       </c>
       <c r="D122" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>17</v>
@@ -4189,75 +4355,104 @@
       </c>
     </row>
     <row r="123" spans="1:9">
-      <c r="A123" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="7"/>
-      <c r="H123" s="7"/>
-      <c r="I123" s="7">
-        <f>ROWS(A122:I122)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" customHeight="1" ht="20">
-      <c r="A124" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="4"/>
-      <c r="I124" s="4"/>
+      <c r="A123" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C123" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D123" s="6">
+        <v>2</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H123" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I123" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C124" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D124" s="6">
+        <v>2</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H124" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="125" spans="1:9">
-      <c r="A125" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D125" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E125" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G125" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H125" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I125" s="5" t="s">
-        <v>13</v>
+      <c r="A125" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C125" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D125" s="6">
+        <v>2</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H125" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="6" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="C126" s="6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D126" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>17</v>
@@ -4277,16 +4472,16 @@
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="6" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="C127" s="6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D127" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>17</v>
@@ -4306,16 +4501,16 @@
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="6" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="C128" s="6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D128" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>17</v>
@@ -4335,16 +4530,16 @@
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="6" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C129" s="6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D129" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>17</v>
@@ -4364,16 +4559,16 @@
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="6" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C130" s="6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D130" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E130" s="6" t="s">
         <v>17</v>
@@ -4392,72 +4587,101 @@
       </c>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
-      <c r="F131" s="7"/>
-      <c r="G131" s="7"/>
-      <c r="H131" s="7"/>
-      <c r="I131" s="7">
-        <f>ROWS(A126:I130)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" customHeight="1" ht="20">
-      <c r="A132" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
+      <c r="A131" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C131" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D131" s="6">
+        <v>2</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G131" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H131" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I131" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C132" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D132" s="6">
+        <v>2</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G132" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H132" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I132" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="133" spans="1:9">
-      <c r="A133" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D133" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E133" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G133" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H133" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I133" s="5" t="s">
-        <v>13</v>
+      <c r="A133" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C133" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D133" s="6">
+        <v>2</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G133" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H133" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I133" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="6" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="C134" s="6">
-        <v>1</v>
+        <v>2015</v>
       </c>
       <c r="D134" s="6">
         <v>2</v>
@@ -4480,166 +4704,1094 @@
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C135" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D135" s="6">
+        <v>2</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G135" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H135" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I135" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
+      <c r="G136" s="7"/>
+      <c r="H136" s="7"/>
+      <c r="I136" s="7">
+        <f>ROWS(A95:I135)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" customHeight="1" ht="20">
+      <c r="A137" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G138" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I138" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C139" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D139" s="6">
+        <v>2</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G139" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H139" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I139" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C140" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D140" s="6">
+        <v>2</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H140" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I140" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C141" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D141" s="6">
+        <v>2</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G141" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H141" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I141" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C142" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D142" s="6">
+        <v>2</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H142" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I142" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C143" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D143" s="6">
+        <v>2</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G143" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H143" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I143" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C144" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D144" s="6">
+        <v>2</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G144" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H144" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I144" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="A145" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C145" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D145" s="6">
+        <v>2</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G145" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H145" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I145" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C146" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D146" s="6">
+        <v>2</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G146" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H146" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I146" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C147" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D147" s="6">
+        <v>2</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G147" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H147" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I147" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
+      <c r="A148" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C148" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D148" s="6">
+        <v>2</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G148" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H148" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I148" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="A149" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C149" s="6">
+        <v>2015</v>
+      </c>
+      <c r="D149" s="6">
+        <v>2</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G149" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H149" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B150" s="7"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="7"/>
+      <c r="G150" s="7"/>
+      <c r="H150" s="7"/>
+      <c r="I150" s="7">
+        <f>ROWS(A139:I149)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" customHeight="1" ht="20">
+      <c r="A151" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B151" s="4"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="4"/>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F152" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G152" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H152" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I152" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="A153" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D153" s="6">
+        <v>1</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G153" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H153" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I153" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D154" s="6">
+        <v>1</v>
+      </c>
+      <c r="E154" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G154" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H154" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I154" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B155" s="7"/>
+      <c r="C155" s="7"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7"/>
+      <c r="G155" s="7"/>
+      <c r="H155" s="7"/>
+      <c r="I155" s="7">
+        <f>ROWS(A153:I154)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" customHeight="1" ht="20">
+      <c r="A156" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="4"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+      <c r="H156" s="4"/>
+      <c r="I156" s="4"/>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G157" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H157" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I157" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C158" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D158" s="6">
+        <v>1</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H158" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I158" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C159" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D159" s="6">
+        <v>1</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G159" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H159" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I159" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="A160" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C160" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D160" s="6">
+        <v>1</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G160" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H160" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I160" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9">
+      <c r="A161" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C161" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D161" s="6">
+        <v>1</v>
+      </c>
+      <c r="E161" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G161" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H161" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I161" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C162" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D162" s="6">
+        <v>1</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G162" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H162" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I162" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B163" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="C163" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D163" s="6">
+        <v>1</v>
+      </c>
+      <c r="E163" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G163" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H163" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I163" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C135" s="6">
+      <c r="B164" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C164" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D164" s="6">
         <v>1</v>
       </c>
-      <c r="D135" s="6">
-        <v>2</v>
-      </c>
-      <c r="E135" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G135" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H135" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I135" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
-      <c r="A136" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B136" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C136" s="6">
+      <c r="E164" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G164" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H164" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I164" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C165" s="6">
+        <v>2016</v>
+      </c>
+      <c r="D165" s="6">
         <v>1</v>
       </c>
-      <c r="D136" s="6">
-        <v>2</v>
-      </c>
-      <c r="E136" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G136" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H136" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I136" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9">
-      <c r="A137" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B137" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C137" s="6">
+      <c r="E165" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G165" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H165" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I165" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B166" s="7"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="7"/>
+      <c r="F166" s="7"/>
+      <c r="G166" s="7"/>
+      <c r="H166" s="7"/>
+      <c r="I166" s="7">
+        <f>ROWS(A158:I165)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" customHeight="1" ht="20">
+      <c r="A167" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B167" s="4"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="4"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="4"/>
+      <c r="I167" s="4"/>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C169" s="6">
         <v>1</v>
       </c>
-      <c r="D137" s="6">
-        <v>2</v>
-      </c>
-      <c r="E137" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G137" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H137" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I137" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
-      <c r="A138" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C138" s="6">
+      <c r="D169" s="6">
+        <v>2</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G169" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H169" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I169" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C170" s="6">
         <v>1</v>
       </c>
-      <c r="D138" s="6">
-        <v>2</v>
-      </c>
-      <c r="E138" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G138" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H138" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I138" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
-      <c r="A139" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-      <c r="G139" s="7"/>
-      <c r="H139" s="7"/>
-      <c r="I139" s="7">
-        <f>ROWS(A134:I138)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9">
-      <c r="A140" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
-      <c r="D140" s="7"/>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="7"/>
-      <c r="H140" s="7"/>
-      <c r="I140" s="7">
-        <f>ROWS(A6:I9) + ROWS(A13:I62) + ROWS(A66:I70) + ROWS(A74:I106) + ROWS(A110:I118) + ROWS(A122:I122) + ROWS(A126:I130) + ROWS(A134:I138)</f>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9">
-      <c r="A141" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
-      <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
-      <c r="G141" s="7"/>
-      <c r="H141" s="7"/>
-      <c r="I141" s="7">
-        <f>ROWS(A6:I9) + ROWS(A13:I62) + ROWS(A66:I70) + ROWS(A74:I106) + ROWS(A110:I118) + ROWS(A122:I122) + ROWS(A126:I130) + ROWS(A134:I138)</f>
-        <v>112</v>
+      <c r="D170" s="6">
+        <v>2</v>
+      </c>
+      <c r="E170" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G170" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H170" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I170" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B171" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C171" s="6">
+        <v>1</v>
+      </c>
+      <c r="D171" s="6">
+        <v>2</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G171" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H171" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I171" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C172" s="6">
+        <v>1</v>
+      </c>
+      <c r="D172" s="6">
+        <v>2</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F172" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G172" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H172" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I172" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B173" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C173" s="6">
+        <v>1</v>
+      </c>
+      <c r="D173" s="6">
+        <v>2</v>
+      </c>
+      <c r="E173" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G173" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H173" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I173" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C174" s="6">
+        <v>1</v>
+      </c>
+      <c r="D174" s="6">
+        <v>2</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G174" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H174" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I174" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B175" s="7"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="7"/>
+      <c r="F175" s="7"/>
+      <c r="G175" s="7"/>
+      <c r="H175" s="7"/>
+      <c r="I175" s="7">
+        <f>ROWS(A169:I174)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B176" s="7"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
+      <c r="G176" s="7"/>
+      <c r="H176" s="7"/>
+      <c r="I176" s="7">
+        <f>ROWS(A6:I12) + ROWS(A16:I82) + ROWS(A86:I91) + ROWS(A95:I135) + ROWS(A139:I149) + ROWS(A153:I154) + ROWS(A158:I165) + ROWS(A169:I174)</f>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9">
+      <c r="A177" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B177" s="7"/>
+      <c r="C177" s="7"/>
+      <c r="D177" s="7"/>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7"/>
+      <c r="H177" s="7"/>
+      <c r="I177" s="7">
+        <f>ROWS(A6:I12) + ROWS(A16:I82) + ROWS(A86:I91) + ROWS(A95:I135) + ROWS(A139:I149) + ROWS(A153:I154) + ROWS(A158:I165) + ROWS(A169:I174)</f>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -4648,23 +5800,23 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A63:H63"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A72:I72"/>
-    <mergeCell ref="A107:H107"/>
-    <mergeCell ref="A108:I108"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="A120:I120"/>
-    <mergeCell ref="A123:H123"/>
-    <mergeCell ref="A124:I124"/>
-    <mergeCell ref="A131:H131"/>
-    <mergeCell ref="A132:I132"/>
-    <mergeCell ref="A139:H139"/>
-    <mergeCell ref="A140:H140"/>
-    <mergeCell ref="A141:H141"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A83:H83"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A92:H92"/>
+    <mergeCell ref="A93:I93"/>
+    <mergeCell ref="A136:H136"/>
+    <mergeCell ref="A137:I137"/>
+    <mergeCell ref="A150:H150"/>
+    <mergeCell ref="A151:I151"/>
+    <mergeCell ref="A155:H155"/>
+    <mergeCell ref="A156:I156"/>
+    <mergeCell ref="A166:H166"/>
+    <mergeCell ref="A167:I167"/>
+    <mergeCell ref="A175:H175"/>
+    <mergeCell ref="A176:H176"/>
+    <mergeCell ref="A177:H177"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>